<commit_message>
Changes: Issues with equation for mu
</commit_message>
<xml_diff>
--- a/Master_Thesis/LacI_TetR_Tup1/PMA1/parameters_0_LacI_TetR_PMA1_model.xlsx
+++ b/Master_Thesis/LacI_TetR_Tup1/PMA1/parameters_0_LacI_TetR_PMA1_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiobroger/Documents/ETH/Master/Master_Thesis/LacI_TetR_Tup1/PMA1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CC9570-50B0-F044-AE9E-B1EB5462F90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B03CF30-C441-E74C-9523-FA9B483A625F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31760" yWindow="500" windowWidth="30240" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="78">
   <si>
     <t>names</t>
   </si>
@@ -252,6 +252,24 @@
   </si>
   <si>
     <t>kL_{PMA1}</t>
+  </si>
+  <si>
+    <t>PMAfactor</t>
+  </si>
+  <si>
+    <t>PMA_factor</t>
+  </si>
+  <si>
+    <t>kLacTetRTup1</t>
+  </si>
+  <si>
+    <t>k_{LacTetRTup1}</t>
+  </si>
+  <si>
+    <t>mufactor</t>
+  </si>
+  <si>
+    <t>mu_factor</t>
   </si>
 </sst>
 </file>
@@ -619,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1482,6 +1500,75 @@
         <v>71</v>
       </c>
     </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="C39" s="2">
+        <v>10</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1</v>
+      </c>
+      <c r="E39" s="2">
+        <v>98</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2">
+        <v>1</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2">
+        <v>1</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes: Code Clean up and clean up of saving structure
</commit_message>
<xml_diff>
--- a/Master_Thesis/LacI_TetR_Tup1/PMA1/parameters_0_LacI_TetR_PMA1_model.xlsx
+++ b/Master_Thesis/LacI_TetR_Tup1/PMA1/parameters_0_LacI_TetR_PMA1_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiobroger/Documents/ETH/Master/Master_Thesis/LacI_TetR_Tup1/PMA1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B03CF30-C441-E74C-9523-FA9B483A625F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E10CB6-E973-9D42-B761-79FBAF693600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31760" yWindow="500" windowWidth="30240" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -798,7 +798,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1">
         <v>0.9</v>
@@ -1051,7 +1051,7 @@
         <v>1E-4</v>
       </c>
       <c r="D18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2">
         <v>0.6</v>
@@ -1074,7 +1074,7 @@
         <v>1E-4</v>
       </c>
       <c r="D19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2">
         <v>0.6</v>
@@ -1350,7 +1350,7 @@
         <v>5</v>
       </c>
       <c r="D31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="2">
         <v>5</v>

</xml_diff>